<commit_message>
Initialization step and get transaction data step updated
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/FrameworkTemplates/REFramework/VB/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\REFramework\RPAChallengeFormFillup\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{669B4AD3-AA49-49D0-BA25-DBEE4D8620D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10248" yWindow="17508" windowWidth="21252" windowHeight="9444" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -160,6 +160,24 @@
   </si>
   <si>
     <t>ProcessABCQueue</t>
+  </si>
+  <si>
+    <t>Data\Data.xlsx</t>
+  </si>
+  <si>
+    <t>FilePath</t>
+  </si>
+  <si>
+    <t>SheetName</t>
+  </si>
+  <si>
+    <t>InputData</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>https://rpachallenge.com/</t>
   </si>
 </sst>
 </file>
@@ -211,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -221,6 +239,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -585,39 +604,132 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
-      <c r="A3" s="2" t="s">
+    <row r="6" spans="1:26" ht="43.2">
+      <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="4" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
-      <c r="A5" t="s">
+    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="28.8">
+      <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1608,6 +1720,9 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
+    <row r="1000" ht="14.25" customHeight="1"/>
+    <row r="1001" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1619,8 +1734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1670,7 +1785,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>25</v>

</xml_diff>